<commit_message>
TC template + review tracker update
Review Tracker:
Update it with amr's reviews.

Test Cases:
Create the template for the sheet
starting in add car feature test cases
</commit_message>
<xml_diff>
--- a/1- PM/review tracker.xlsx
+++ b/1- PM/review tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\Car-Purchasing-App\1- PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beshoy Sameh\Documents\GitHub\Car-Purchasing-App\1- PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAE1C3A-07C3-4B84-80F3-A8305A10B153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9950C8D-2AB7-4A19-8552-149AB52F1883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>review TRACKER</t>
   </si>
@@ -162,6 +162,25 @@
   </si>
   <si>
     <t>1. Add id to the alternative flows.                                                  2. Add functional reqirments to "View car list".                       3. Edit the output for delete and reserved car features.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review </t>
+  </si>
+  <si>
+    <t>Each task from the team , coach and Eng/ moahmed hassan should has review.</t>
+  </si>
+  <si>
+    <t>RTM</t>
+  </si>
+  <si>
+    <t>1. update all use cases.
+2. Add alternative  flows from srs.</t>
+  </si>
+  <si>
+    <t>Add ids to be reahable.</t>
+  </si>
+  <si>
+    <t>change "manage" relation to be add/delete.</t>
   </si>
 </sst>
 </file>
@@ -532,15 +551,15 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,8 +927,8 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -933,13 +952,13 @@
     </row>
     <row r="2" spans="1:7" ht="44.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="49"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1">
@@ -1027,7 +1046,7 @@
       </c>
       <c r="G7" s="25"/>
     </row>
-    <row r="8" spans="1:7" ht="12.75">
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="26"/>
       <c r="B8" s="27"/>
       <c r="C8" s="28"/>
@@ -1055,7 +1074,7 @@
       </c>
       <c r="G9" s="35"/>
     </row>
-    <row r="10" spans="1:7" ht="51">
+    <row r="10" spans="1:7" ht="60">
       <c r="A10" s="36"/>
       <c r="B10" s="36" t="s">
         <v>18</v>
@@ -1074,7 +1093,7 @@
       </c>
       <c r="G10" s="38"/>
     </row>
-    <row r="11" spans="1:7" ht="38.25">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="32"/>
       <c r="B11" s="32" t="s">
         <v>14</v>
@@ -1093,7 +1112,7 @@
       </c>
       <c r="G11" s="39"/>
     </row>
-    <row r="12" spans="1:7" ht="12.75">
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" s="26"/>
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
@@ -1202,7 +1221,7 @@
       <c r="B18" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="48" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="32" t="s">
@@ -1216,43 +1235,75 @@
       </c>
       <c r="G18" s="40"/>
     </row>
-    <row r="19" spans="1:7" ht="15">
+    <row r="19" spans="1:7" ht="48.75" customHeight="1">
       <c r="A19" s="32"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="40"/>
+      <c r="B19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="39">
+        <v>45082</v>
+      </c>
       <c r="G19" s="40"/>
     </row>
-    <row r="20" spans="1:7" ht="12.75">
+    <row r="20" spans="1:7" ht="30">
       <c r="A20" s="32"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="40"/>
+      <c r="B20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="39">
+        <v>45082</v>
+      </c>
       <c r="G20" s="40"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75">
+    <row r="21" spans="1:7" ht="22.5" customHeight="1">
       <c r="A21" s="32"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="40"/>
+      <c r="B21" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="39">
+        <v>45082</v>
+      </c>
       <c r="G21" s="41"/>
     </row>
-    <row r="22" spans="1:7" ht="12.75">
+    <row r="22" spans="1:7" ht="15">
       <c r="A22" s="32"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="40"/>
+      <c r="B22" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="39">
+        <v>45082</v>
+      </c>
       <c r="G22" s="41"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75">
+    <row r="23" spans="1:7" ht="15">
       <c r="A23" s="32"/>
       <c r="B23" s="41"/>
       <c r="C23" s="42"/>
@@ -1261,7 +1312,7 @@
       <c r="F23" s="40"/>
       <c r="G23" s="41"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75">
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" s="41"/>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
@@ -1270,7 +1321,7 @@
       <c r="F24" s="40"/>
       <c r="G24" s="41"/>
     </row>
-    <row r="25" spans="1:7" ht="12.75">
+    <row r="25" spans="1:7" ht="15">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
@@ -1279,7 +1330,7 @@
       <c r="F25" s="40"/>
       <c r="G25" s="41"/>
     </row>
-    <row r="26" spans="1:7" ht="12.75">
+    <row r="26" spans="1:7" ht="15">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="42"/>
@@ -1288,7 +1339,7 @@
       <c r="F26" s="40"/>
       <c r="G26" s="41"/>
     </row>
-    <row r="27" spans="1:7" ht="12.75">
+    <row r="27" spans="1:7" ht="15">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="42"/>
@@ -1297,7 +1348,7 @@
       <c r="F27" s="40"/>
       <c r="G27" s="41"/>
     </row>
-    <row r="28" spans="1:7" ht="12.75">
+    <row r="28" spans="1:7" ht="15">
       <c r="A28" s="41"/>
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
@@ -1306,7 +1357,7 @@
       <c r="F28" s="40"/>
       <c r="G28" s="41"/>
     </row>
-    <row r="29" spans="1:7" ht="12.75">
+    <row r="29" spans="1:7" ht="15">
       <c r="A29" s="41"/>
       <c r="B29" s="41"/>
       <c r="C29" s="42"/>
@@ -1315,7 +1366,7 @@
       <c r="F29" s="40"/>
       <c r="G29" s="41"/>
     </row>
-    <row r="30" spans="1:7" ht="12.75">
+    <row r="30" spans="1:7" ht="15">
       <c r="A30" s="41"/>
       <c r="B30" s="41"/>
       <c r="C30" s="42"/>
@@ -1324,7 +1375,7 @@
       <c r="F30" s="40"/>
       <c r="G30" s="41"/>
     </row>
-    <row r="31" spans="1:7" ht="12.75">
+    <row r="31" spans="1:7" ht="15">
       <c r="A31" s="41"/>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
@@ -1333,7 +1384,7 @@
       <c r="F31" s="40"/>
       <c r="G31" s="41"/>
     </row>
-    <row r="32" spans="1:7" ht="12.75">
+    <row r="32" spans="1:7" ht="15">
       <c r="A32" s="41"/>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
@@ -1342,7 +1393,7 @@
       <c r="F32" s="40"/>
       <c r="G32" s="41"/>
     </row>
-    <row r="33" spans="1:7" ht="12.75">
+    <row r="33" spans="1:7" ht="15">
       <c r="A33" s="41"/>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
@@ -1351,7 +1402,7 @@
       <c r="F33" s="40"/>
       <c r="G33" s="41"/>
     </row>
-    <row r="34" spans="1:7" ht="12.75">
+    <row r="34" spans="1:7" ht="15">
       <c r="A34" s="41"/>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
@@ -1360,7 +1411,7 @@
       <c r="F34" s="40"/>
       <c r="G34" s="41"/>
     </row>
-    <row r="35" spans="1:7" ht="12.75">
+    <row r="35" spans="1:7" ht="15">
       <c r="A35" s="41"/>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
@@ -1369,7 +1420,7 @@
       <c r="F35" s="40"/>
       <c r="G35" s="41"/>
     </row>
-    <row r="36" spans="1:7" ht="12.75">
+    <row r="36" spans="1:7" ht="15">
       <c r="A36" s="41"/>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
@@ -1378,7 +1429,7 @@
       <c r="F36" s="40"/>
       <c r="G36" s="41"/>
     </row>
-    <row r="37" spans="1:7" ht="12.75">
+    <row r="37" spans="1:7" ht="15">
       <c r="A37" s="41"/>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
@@ -1387,7 +1438,7 @@
       <c r="F37" s="40"/>
       <c r="G37" s="41"/>
     </row>
-    <row r="38" spans="1:7" ht="12.75">
+    <row r="38" spans="1:7" ht="15">
       <c r="A38" s="41"/>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
@@ -1396,7 +1447,7 @@
       <c r="F38" s="40"/>
       <c r="G38" s="41"/>
     </row>
-    <row r="39" spans="1:7" ht="12.75" hidden="1">
+    <row r="39" spans="1:7" ht="15" hidden="1">
       <c r="A39" s="44"/>
       <c r="B39" s="44"/>
       <c r="C39" s="45"/>

</xml_diff>